<commit_message>
Added link to Grupo 4 Github project page
</commit_message>
<xml_diff>
--- a/SIGA - Equipes - LES - 5 (M) ADS - 2S2021.xlsx
+++ b/SIGA - Equipes - LES - 5 (M) ADS - 2S2021.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anderson\Carreira Docente\2021\FATEC - CPS\FATEC2021-2 - LabEngSW - ADS - Matutino\Projetos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fábio Carvalho\Documents\Fatec\FATEC_CPS_ADS_2S2021_5M_LES_Projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ADB28E-275C-4310-9E00-B228CAE0143D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADS-5M-LES - Entregas" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ADS-5M-LES - Entregas'!$A$5:$P$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ADS-5M-LES - Equipes e Temas'!$A$5:$G$29</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="111">
   <si>
     <t>FATEC CAMPINAS - ADS-5M-LES - LABORATÓRIO DE ENGENHARIA DE SOFTWARE</t>
   </si>
@@ -362,12 +363,18 @@
   </si>
   <si>
     <t>Projetos - v. 09.agosto.2021</t>
+  </si>
+  <si>
+    <t>Murilo Damario</t>
+  </si>
+  <si>
+    <t>E-commerce - Loja de Roupas de Marca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
@@ -639,7 +646,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -916,14 +923,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1729,10 +1736,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1958,7 +1965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2563,8 +2570,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:G29">
-    <sortState ref="A6:G29">
+  <autoFilter ref="A5:G29" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:G29">
       <sortCondition ref="C6:C29"/>
       <sortCondition ref="B6:B29"/>
     </sortState>
@@ -2575,17 +2582,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="70c83078-cc4d-40bc-85b2-115ccd37b395">
-      <UserInfo>
-        <DisplayName>Banco de Dados-A-M-ANALISE E DESENV. DE SISTEMAS-276-20212 Members</DisplayName>
-        <AccountId>39</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2754,27 +2756,23 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="70c83078-cc4d-40bc-85b2-115ccd37b395">
+      <UserInfo>
+        <DisplayName>Banco de Dados-A-M-ANALISE E DESENV. DE SISTEMAS-276-20212 Members</DisplayName>
+        <AccountId>39</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{764CCD6E-DC5A-4481-80F8-06C3FB450BA8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE010457-3936-42D9-9416-4419188BE90C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="23e7ea15-7176-4ddd-bf4e-71ba86a8c6f1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="70c83078-cc4d-40bc-85b2-115ccd37b395"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2799,9 +2797,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE010457-3936-42D9-9416-4419188BE90C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{764CCD6E-DC5A-4481-80F8-06C3FB450BA8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="23e7ea15-7176-4ddd-bf4e-71ba86a8c6f1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="70c83078-cc4d-40bc-85b2-115ccd37b395"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>